<commit_message>
Addressed several tabular data issues
</commit_message>
<xml_diff>
--- a/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
+++ b/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
@@ -5,19 +5,19 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krautscheid/git/vrdr-dotnet/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rscalfani/Documents/code/NVSS/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1700D00C-B164-A748-B4CF-19E68D35B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C458F75-F412-3245-9CDD-2129125E0949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2980" yWindow="7940" windowWidth="25600" windowHeight="20500" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="51200" windowHeight="28320" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality_Trim_mappings" sheetId="2" r:id="rId1"/>
     <sheet name="Mortality_Full_Details" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mortality_Full_Details!$B$2:$Q$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mortality_Full_Details!$A$1:$K$260</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Mortality_Full_Details!$A$1:$G$260</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Mortality_Full_Details!$1:$1</definedName>
     <definedName name="Z_F1069C25_F3CC_400B_8C16_E88E31027CCC_.wvu.FilterData" localSheetId="1" hidden="1">Mortality_Full_Details!$B$2:$Q$260</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="753">
   <si>
     <t>Field #</t>
   </si>
@@ -2628,6 +2628,18 @@
   <si>
     <t>SPOUSEL</t>
   </si>
+  <si>
+    <t>two_digit_country</t>
+  </si>
+  <si>
+    <t>Time of Injury Modifier</t>
+  </si>
+  <si>
+    <t>full_state_name</t>
+  </si>
+  <si>
+    <t>toi_unit_modifier</t>
+  </si>
 </sst>
 </file>
 
@@ -2636,7 +2648,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2698,6 +2710,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Sans-serif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2767,7 +2785,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2950,13 +2968,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="45" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3304,8 +3323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD74E696-0F05-DF43-9EB9-28DAB6A6F493}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3593,7 +3612,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>200</v>
@@ -3611,7 +3630,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>201</v>
@@ -3629,7 +3648,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>204</v>
@@ -3647,7 +3666,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>205</v>
@@ -3665,7 +3684,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>209</v>
@@ -3683,7 +3702,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>211</v>
@@ -3701,7 +3720,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>213</v>
@@ -3718,8 +3737,11 @@
       <c r="E23" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="68" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>215</v>
@@ -3737,7 +3759,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>217</v>
@@ -3755,7 +3777,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>222</v>
@@ -3773,7 +3795,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>225</v>
@@ -3791,7 +3813,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>227</v>
@@ -3809,7 +3831,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>229</v>
@@ -3827,7 +3849,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>230</v>
@@ -3845,7 +3867,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>231</v>
@@ -3863,7 +3885,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>232</v>
@@ -5271,11 +5293,11 @@
       <c r="C109" t="s">
         <v>243</v>
       </c>
-      <c r="D109" t="s">
-        <v>707</v>
-      </c>
-      <c r="E109" t="s">
-        <v>727</v>
+      <c r="D109" s="68" t="s">
+        <v>630</v>
+      </c>
+      <c r="F109" s="68" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -5332,7 +5354,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:7">
       <c r="A113">
         <f t="shared" si="2"/>
         <v>979</v>
@@ -5350,7 +5372,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:7">
       <c r="A114">
         <f t="shared" si="2"/>
         <v>980</v>
@@ -5368,7 +5390,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:7">
       <c r="A115">
         <f t="shared" si="2"/>
         <v>981</v>
@@ -5386,7 +5408,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:7">
       <c r="A116">
         <f t="shared" si="2"/>
         <v>983</v>
@@ -5404,7 +5426,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:7">
       <c r="A117">
         <f t="shared" si="2"/>
         <v>985</v>
@@ -5422,7 +5444,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:7">
       <c r="A118">
         <f t="shared" si="2"/>
         <v>989</v>
@@ -5440,7 +5462,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:7">
       <c r="A119">
         <f t="shared" si="2"/>
         <v>993</v>
@@ -5458,7 +5480,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:7">
       <c r="A120">
         <f t="shared" si="2"/>
         <v>994</v>
@@ -5476,7 +5498,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:7">
       <c r="A121">
         <f t="shared" si="2"/>
         <v>1024</v>
@@ -5494,7 +5516,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:7">
       <c r="A122">
         <f t="shared" si="2"/>
         <v>1025</v>
@@ -5512,7 +5534,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:7">
       <c r="A123">
         <f t="shared" si="2"/>
         <v>1037</v>
@@ -5530,7 +5552,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:7">
       <c r="A124">
         <f t="shared" si="2"/>
         <v>1067</v>
@@ -5548,7 +5570,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:7">
       <c r="A125">
         <f t="shared" si="2"/>
         <v>1069</v>
@@ -5566,7 +5588,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:7">
       <c r="A126">
         <f t="shared" si="2"/>
         <v>1071</v>
@@ -5584,24 +5606,27 @@
         <v>706</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:7" ht="15">
       <c r="A127">
         <v>1075</v>
       </c>
       <c r="B127">
         <v>1</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="68" t="s">
         <v>282</v>
       </c>
-      <c r="D127" t="s">
-        <v>630</v>
-      </c>
-      <c r="F127" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="D127" s="71" t="s">
+        <v>750</v>
+      </c>
+      <c r="E127" s="68" t="s">
+        <v>727</v>
+      </c>
+      <c r="G127" s="68" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128">
         <v>1076</v>
       </c>
@@ -5906,7 +5931,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:7">
       <c r="A145">
         <f t="shared" si="3"/>
         <v>1385</v>
@@ -5917,11 +5942,11 @@
       <c r="C145" t="s">
         <v>329</v>
       </c>
-      <c r="D145" s="70" t="s">
+      <c r="D145" s="68" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:7">
       <c r="A146">
         <f t="shared" si="3"/>
         <v>1435</v>
@@ -5929,14 +5954,14 @@
       <c r="B146">
         <v>50</v>
       </c>
-      <c r="C146" s="70" t="s">
+      <c r="C146" s="68" t="s">
         <v>748</v>
       </c>
-      <c r="D146" s="70" t="s">
+      <c r="D146" s="68" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:7">
       <c r="A147">
         <f t="shared" si="3"/>
         <v>1485</v>
@@ -5951,7 +5976,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:7">
       <c r="A148">
         <f t="shared" si="3"/>
         <v>1495</v>
@@ -5969,7 +5994,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:7">
       <c r="A149">
         <f t="shared" si="3"/>
         <v>1505</v>
@@ -5984,7 +6009,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:7">
       <c r="A150">
         <f t="shared" si="3"/>
         <v>1533</v>
@@ -5999,7 +6024,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:7">
       <c r="A151">
         <f t="shared" si="3"/>
         <v>1543</v>
@@ -6017,7 +6042,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:7">
       <c r="A152">
         <f t="shared" si="3"/>
         <v>1553</v>
@@ -6032,7 +6057,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:7">
       <c r="A153">
         <f t="shared" si="3"/>
         <v>1560</v>
@@ -6047,7 +6072,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:7">
       <c r="A154">
         <f t="shared" si="3"/>
         <v>1588</v>
@@ -6065,7 +6090,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:7">
       <c r="A155">
         <f t="shared" si="3"/>
         <v>1597</v>
@@ -6083,7 +6108,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:7">
       <c r="A156">
         <f t="shared" si="3"/>
         <v>1625</v>
@@ -6100,8 +6125,11 @@
       <c r="E156" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="G156" s="68" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157">
         <f t="shared" si="3"/>
         <v>1653</v>
@@ -6119,7 +6147,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:7">
       <c r="A158">
         <f t="shared" si="3"/>
         <v>1681</v>
@@ -6134,7 +6162,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:7">
       <c r="A159">
         <f t="shared" si="3"/>
         <v>1731</v>
@@ -6152,7 +6180,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:7">
       <c r="A160">
         <f t="shared" si="3"/>
         <v>1733</v>
@@ -7226,7 +7254,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="225" spans="1:6">
+    <row r="225" spans="1:7">
       <c r="A225">
         <f t="shared" ref="A225:A230" si="6">A224+B224</f>
         <v>4062</v>
@@ -7241,7 +7269,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:7">
       <c r="A226">
         <f t="shared" si="6"/>
         <v>4072</v>
@@ -7259,7 +7287,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="227" spans="1:6">
+    <row r="227" spans="1:7">
       <c r="A227">
         <f t="shared" si="6"/>
         <v>4082</v>
@@ -7274,7 +7302,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:7">
       <c r="A228">
         <f t="shared" si="6"/>
         <v>4110</v>
@@ -7289,7 +7317,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="229" spans="1:6">
+    <row r="229" spans="1:7">
       <c r="A229">
         <f t="shared" si="6"/>
         <v>4120</v>
@@ -7307,7 +7335,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="230" spans="1:6">
+    <row r="230" spans="1:7">
       <c r="A230">
         <f t="shared" si="6"/>
         <v>4130</v>
@@ -7322,7 +7350,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="231" spans="1:6">
+    <row r="231" spans="1:7">
       <c r="A231">
         <v>4137</v>
       </c>
@@ -7336,7 +7364,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="232" spans="1:6">
+    <row r="232" spans="1:7">
       <c r="A232">
         <v>4187</v>
       </c>
@@ -7350,7 +7378,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:7">
       <c r="A233">
         <v>4215</v>
       </c>
@@ -7364,7 +7392,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:7">
       <c r="A234">
         <v>4217</v>
       </c>
@@ -7378,7 +7406,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="235" spans="1:6">
+    <row r="235" spans="1:7">
       <c r="A235">
         <v>4245</v>
       </c>
@@ -7392,7 +7420,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:7">
       <c r="A236">
         <v>4254</v>
       </c>
@@ -7409,7 +7437,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:7">
       <c r="A237">
         <v>4262</v>
       </c>
@@ -7426,7 +7454,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="238" spans="1:6">
+    <row r="238" spans="1:7">
       <c r="A238">
         <v>4270</v>
       </c>
@@ -7443,7 +7471,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="239" spans="1:6">
+    <row r="239" spans="1:7">
       <c r="A239">
         <v>4298</v>
       </c>
@@ -7459,8 +7487,11 @@
       <c r="E239" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="240" spans="1:6">
+      <c r="G239" s="68" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
       <c r="A240">
         <f>A239+B239</f>
         <v>4326</v>
@@ -7488,7 +7519,7 @@
       <c r="C241" t="s">
         <v>555</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D241" s="68" t="s">
         <v>630</v>
       </c>
       <c r="F241" t="s">
@@ -7830,8 +7861,8 @@
   </sheetPr>
   <dimension ref="A1:L1048511"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="K147" sqref="K147"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -7841,8 +7872,9 @@
     <col min="3" max="3" width="8.1640625" style="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" style="11" customWidth="1"/>
     <col min="5" max="5" width="19.5" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.1640625" style="11" customWidth="1"/>
-    <col min="7" max="8" width="13" style="7" customWidth="1"/>
+    <col min="6" max="6" width="29.5" style="11" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13" style="7" customWidth="1"/>
     <col min="9" max="9" width="9" style="7" customWidth="1"/>
     <col min="10" max="10" width="15.5" style="7" customWidth="1"/>
     <col min="11" max="11" width="30.6640625" style="10" customWidth="1"/>
@@ -9800,7 +9832,7 @@
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="D68" s="68" t="s">
+      <c r="D68" s="69" t="s">
         <v>168</v>
       </c>
       <c r="E68" s="8" t="s">
@@ -9831,7 +9863,7 @@
       <c r="C69" s="6">
         <v>3</v>
       </c>
-      <c r="D69" s="68"/>
+      <c r="D69" s="69"/>
       <c r="E69" s="8" t="s">
         <v>171</v>
       </c>
@@ -9860,7 +9892,7 @@
       <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="D70" s="68"/>
+      <c r="D70" s="69"/>
       <c r="E70" s="8" t="s">
         <v>173</v>
       </c>
@@ -9889,7 +9921,7 @@
       <c r="C71" s="6">
         <v>3</v>
       </c>
-      <c r="D71" s="68"/>
+      <c r="D71" s="69"/>
       <c r="E71" s="8" t="s">
         <v>174</v>
       </c>
@@ -9918,7 +9950,7 @@
       <c r="C72" s="6">
         <v>3</v>
       </c>
-      <c r="D72" s="68"/>
+      <c r="D72" s="69"/>
       <c r="E72" s="8" t="s">
         <v>175</v>
       </c>
@@ -9947,7 +9979,7 @@
       <c r="C73" s="6">
         <v>3</v>
       </c>
-      <c r="D73" s="68"/>
+      <c r="D73" s="69"/>
       <c r="E73" s="8" t="s">
         <v>176</v>
       </c>
@@ -9976,7 +10008,7 @@
       <c r="C74" s="6">
         <v>3</v>
       </c>
-      <c r="D74" s="68"/>
+      <c r="D74" s="69"/>
       <c r="E74" s="8" t="s">
         <v>177</v>
       </c>
@@ -10005,7 +10037,7 @@
       <c r="C75" s="6">
         <v>3</v>
       </c>
-      <c r="D75" s="68"/>
+      <c r="D75" s="69"/>
       <c r="E75" s="8" t="s">
         <v>178</v>
       </c>
@@ -10034,7 +10066,7 @@
       <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="D76" s="68"/>
+      <c r="D76" s="69"/>
       <c r="E76" s="8" t="s">
         <v>179</v>
       </c>
@@ -10063,7 +10095,7 @@
       <c r="C77" s="6">
         <v>3</v>
       </c>
-      <c r="D77" s="68"/>
+      <c r="D77" s="69"/>
       <c r="E77" s="8" t="s">
         <v>180</v>
       </c>
@@ -10092,7 +10124,7 @@
       <c r="C78" s="6">
         <v>3</v>
       </c>
-      <c r="D78" s="68"/>
+      <c r="D78" s="69"/>
       <c r="E78" s="8" t="s">
         <v>181</v>
       </c>
@@ -10121,7 +10153,7 @@
       <c r="C79" s="6">
         <v>3</v>
       </c>
-      <c r="D79" s="68"/>
+      <c r="D79" s="69"/>
       <c r="E79" s="8" t="s">
         <v>182</v>
       </c>
@@ -10150,7 +10182,7 @@
       <c r="C80" s="6">
         <v>3</v>
       </c>
-      <c r="D80" s="68"/>
+      <c r="D80" s="69"/>
       <c r="E80" s="8" t="s">
         <v>183</v>
       </c>
@@ -10179,7 +10211,7 @@
       <c r="C81" s="6">
         <v>3</v>
       </c>
-      <c r="D81" s="68"/>
+      <c r="D81" s="69"/>
       <c r="E81" s="8" t="s">
         <v>184</v>
       </c>
@@ -10208,7 +10240,7 @@
       <c r="C82" s="6">
         <v>3</v>
       </c>
-      <c r="D82" s="68"/>
+      <c r="D82" s="69"/>
       <c r="E82" s="8" t="s">
         <v>185</v>
       </c>
@@ -10237,7 +10269,7 @@
       <c r="C83" s="6">
         <v>3</v>
       </c>
-      <c r="D83" s="68"/>
+      <c r="D83" s="69"/>
       <c r="E83" s="8" t="s">
         <v>186</v>
       </c>
@@ -10798,7 +10830,7 @@
       <c r="F101" s="22" t="s">
         <v>685</v>
       </c>
-      <c r="G101" s="69" t="s">
+      <c r="G101" s="70" t="s">
         <v>227</v>
       </c>
       <c r="H101" s="20" t="s">
@@ -10829,7 +10861,7 @@
       <c r="F102" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G102" s="69"/>
+      <c r="G102" s="70"/>
       <c r="H102" s="33"/>
       <c r="I102" s="7" t="s">
         <v>706</v>
@@ -10861,7 +10893,7 @@
       <c r="F103" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G103" s="69"/>
+      <c r="G103" s="70"/>
       <c r="H103" s="33"/>
       <c r="I103" s="7" t="s">
         <v>706</v>
@@ -10892,7 +10924,7 @@
       <c r="F104" s="22" t="s">
         <v>686</v>
       </c>
-      <c r="G104" s="69"/>
+      <c r="G104" s="70"/>
       <c r="H104" s="20" t="s">
         <v>727</v>
       </c>
@@ -10923,7 +10955,7 @@
       <c r="F105" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="G105" s="69"/>
+      <c r="G105" s="70"/>
       <c r="H105" s="20" t="s">
         <v>727</v>
       </c>
@@ -10952,7 +10984,7 @@
       <c r="F106" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G106" s="69"/>
+      <c r="G106" s="70"/>
       <c r="H106" s="33"/>
       <c r="I106" s="33" t="s">
         <v>706</v>
@@ -10983,7 +11015,7 @@
       <c r="F107" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G107" s="69"/>
+      <c r="G107" s="70"/>
       <c r="H107" s="33"/>
       <c r="I107" s="33" t="s">
         <v>706</v>
@@ -11014,7 +11046,7 @@
       <c r="F108" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G108" s="69"/>
+      <c r="G108" s="70"/>
       <c r="H108" s="33"/>
       <c r="I108" s="33" t="s">
         <v>706</v>
@@ -11045,7 +11077,7 @@
       <c r="F109" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="G109" s="69"/>
+      <c r="G109" s="70"/>
       <c r="H109" s="20" t="s">
         <v>727</v>
       </c>
@@ -11076,7 +11108,7 @@
       <c r="F110" s="22" t="s">
         <v>689</v>
       </c>
-      <c r="G110" s="69"/>
+      <c r="G110" s="70"/>
       <c r="H110" s="20" t="s">
         <v>727</v>
       </c>
@@ -11105,7 +11137,7 @@
       <c r="F111" s="22" t="s">
         <v>690</v>
       </c>
-      <c r="G111" s="69"/>
+      <c r="G111" s="70"/>
       <c r="H111" s="20" t="s">
         <v>727</v>
       </c>
@@ -11134,7 +11166,7 @@
       <c r="F112" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="G112" s="69"/>
+      <c r="G112" s="70"/>
       <c r="H112" s="20" t="s">
         <v>727</v>
       </c>
@@ -11163,7 +11195,7 @@
       <c r="F113" s="22" t="s">
         <v>692</v>
       </c>
-      <c r="G113" s="69"/>
+      <c r="G113" s="70"/>
       <c r="H113" s="20" t="s">
         <v>727</v>
       </c>
@@ -11192,7 +11224,7 @@
       <c r="F114" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G114" s="69"/>
+      <c r="G114" s="70"/>
       <c r="H114" s="33"/>
       <c r="I114" s="33" t="s">
         <v>706</v>
@@ -11221,7 +11253,7 @@
       <c r="F115" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="G115" s="69"/>
+      <c r="G115" s="70"/>
       <c r="H115" s="20" t="s">
         <v>727</v>
       </c>
@@ -11250,7 +11282,7 @@
       <c r="F116" s="22" t="s">
         <v>694</v>
       </c>
-      <c r="G116" s="69"/>
+      <c r="G116" s="70"/>
       <c r="H116" s="20" t="s">
         <v>727</v>
       </c>
@@ -11279,7 +11311,7 @@
       <c r="F117" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="G117" s="69"/>
+      <c r="G117" s="70"/>
       <c r="H117" s="20"/>
       <c r="I117" s="33">
         <v>2022</v>
@@ -11310,7 +11342,7 @@
       <c r="F118" s="22" t="s">
         <v>695</v>
       </c>
-      <c r="G118" s="69"/>
+      <c r="G118" s="70"/>
       <c r="H118" s="20" t="s">
         <v>727</v>
       </c>
@@ -11339,7 +11371,7 @@
       <c r="F119" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="G119" s="69"/>
+      <c r="G119" s="70"/>
       <c r="H119" s="20" t="s">
         <v>727</v>
       </c>
@@ -11368,7 +11400,7 @@
       <c r="F120" s="22" t="s">
         <v>696</v>
       </c>
-      <c r="G120" s="69"/>
+      <c r="G120" s="70"/>
       <c r="H120" s="20" t="s">
         <v>727</v>
       </c>
@@ -11397,7 +11429,7 @@
       <c r="F121" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G121" s="69"/>
+      <c r="G121" s="70"/>
       <c r="H121" s="33"/>
       <c r="I121" s="33" t="s">
         <v>706</v>
@@ -11427,7 +11459,7 @@
       <c r="F122" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G122" s="69"/>
+      <c r="G122" s="70"/>
       <c r="H122" s="33"/>
       <c r="I122" s="33" t="s">
         <v>706</v>
@@ -12400,9 +12432,7 @@
       <c r="E156" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="F156" s="1" t="s">
-        <v>642</v>
-      </c>
+      <c r="F156" s="1"/>
       <c r="G156" s="20" t="s">
         <v>310</v>
       </c>
@@ -14732,7 +14762,7 @@
         <v>555</v>
       </c>
       <c r="F241" s="11" t="s">
-        <v>630</v>
+        <v>727</v>
       </c>
       <c r="G241" s="7" t="s">
         <v>556</v>
@@ -15312,26 +15342,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d8a0f530da2fdbe2e55626e9ad23fb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d278552e3c3a0a08e9db34919b560943" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -15553,30 +15567,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0A455F-891F-4D48-ABA8-1B564ACEA7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15596,10 +15615,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added special case mappings
</commit_message>
<xml_diff>
--- a/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
+++ b/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rscalfani/Documents/code/NVSS/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C458F75-F412-3245-9CDD-2129125E0949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A281594E-EE57-C946-A648-86809F3FEF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="51200" windowHeight="28320" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mortality_Trim_mappings" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mortality_Full_Details!$A$1:$K$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mortality_Trim_mappings!$A$1:$G$260</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Mortality_Full_Details!$A$1:$G$260</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Mortality_Full_Details!$1:$1</definedName>
     <definedName name="Z_F1069C25_F3CC_400B_8C16_E88E31027CCC_.wvu.FilterData" localSheetId="1" hidden="1">Mortality_Full_Details!$B$2:$Q$260</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1984" uniqueCount="761">
   <si>
     <t>Field #</t>
   </si>
@@ -2639,6 +2640,30 @@
   </si>
   <si>
     <t>toi_unit_modifier</t>
+  </si>
+  <si>
+    <t>Certifier Not Found</t>
+  </si>
+  <si>
+    <t>county_code_to_name</t>
+  </si>
+  <si>
+    <t>Date Received</t>
+  </si>
+  <si>
+    <t>extract_month</t>
+  </si>
+  <si>
+    <t>extract_day</t>
+  </si>
+  <si>
+    <t>reuse_certstatecd</t>
+  </si>
+  <si>
+    <t>reuse_funstatecd</t>
+  </si>
+  <si>
+    <t>capitalize_first_letter</t>
   </si>
 </sst>
 </file>
@@ -2969,13 +2994,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" textRotation="45" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3323,8 +3348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD74E696-0F05-DF43-9EB9-28DAB6A6F493}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5067,7 +5092,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:7">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>689</v>
@@ -5085,7 +5110,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:7">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>693</v>
@@ -5097,13 +5122,16 @@
         <v>219</v>
       </c>
       <c r="D98" t="s">
-        <v>630</v>
-      </c>
-      <c r="F98" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <v>755</v>
+      </c>
+      <c r="E98" s="68" t="s">
+        <v>727</v>
+      </c>
+      <c r="G98" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>695</v>
@@ -5115,13 +5143,16 @@
         <v>222</v>
       </c>
       <c r="D99" t="s">
-        <v>630</v>
-      </c>
-      <c r="F99" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+        <v>755</v>
+      </c>
+      <c r="E99" s="68" t="s">
+        <v>727</v>
+      </c>
+      <c r="G99" s="68" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>697</v>
@@ -5139,7 +5170,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:7">
       <c r="A101">
         <v>701</v>
       </c>
@@ -5156,7 +5187,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:7">
       <c r="A102">
         <f>A101+B101</f>
         <v>702</v>
@@ -5174,7 +5205,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:7">
       <c r="A103">
         <f t="shared" ref="A103:A126" si="2">A102+B102</f>
         <v>703</v>
@@ -5192,7 +5223,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:7">
       <c r="A104">
         <f t="shared" si="2"/>
         <v>704</v>
@@ -5210,7 +5241,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:7">
       <c r="A105">
         <f t="shared" si="2"/>
         <v>705</v>
@@ -5228,7 +5259,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:7">
       <c r="A106">
         <f t="shared" si="2"/>
         <v>710</v>
@@ -5246,7 +5277,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:7">
       <c r="A107">
         <f t="shared" si="2"/>
         <v>715</v>
@@ -5264,7 +5295,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:7">
       <c r="A108">
         <f t="shared" si="2"/>
         <v>875</v>
@@ -5282,7 +5313,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:7">
       <c r="A109">
         <f t="shared" si="2"/>
         <v>876</v>
@@ -5300,7 +5331,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:7">
       <c r="A110">
         <f t="shared" si="2"/>
         <v>976</v>
@@ -5318,7 +5349,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:7">
       <c r="A111">
         <f t="shared" si="2"/>
         <v>977</v>
@@ -5336,7 +5367,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:7">
       <c r="A112">
         <f t="shared" si="2"/>
         <v>978</v>
@@ -5491,11 +5522,11 @@
       <c r="C120" t="s">
         <v>265</v>
       </c>
-      <c r="D120" t="s">
-        <v>696</v>
-      </c>
-      <c r="E120" t="s">
-        <v>727</v>
+      <c r="D120" s="68" t="s">
+        <v>630</v>
+      </c>
+      <c r="F120" s="68" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -5616,7 +5647,7 @@
       <c r="C127" s="68" t="s">
         <v>282</v>
       </c>
-      <c r="D127" s="71" t="s">
+      <c r="D127" s="69" t="s">
         <v>750</v>
       </c>
       <c r="E127" s="68" t="s">
@@ -5643,7 +5674,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:7">
       <c r="A129">
         <f>A128+B128</f>
         <v>1081</v>
@@ -5661,7 +5692,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:7">
       <c r="A130">
         <f t="shared" ref="A130:A185" si="3">A129+B129</f>
         <v>1082</v>
@@ -5679,7 +5710,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:7">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>1112</v>
@@ -5697,7 +5728,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:7">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>1162</v>
@@ -5715,7 +5746,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:7">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>1172</v>
@@ -5733,7 +5764,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:7">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>1182</v>
@@ -5751,7 +5782,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:7">
       <c r="A135">
         <f t="shared" si="3"/>
         <v>1232</v>
@@ -5769,7 +5800,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:7">
       <c r="A136">
         <f t="shared" si="3"/>
         <v>1242</v>
@@ -5787,7 +5818,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:7">
       <c r="A137">
         <f t="shared" si="3"/>
         <v>1252</v>
@@ -5805,7 +5836,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:7">
       <c r="A138">
         <f t="shared" si="3"/>
         <v>1280</v>
@@ -5822,8 +5853,11 @@
       <c r="E138" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="G138" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
       <c r="A139">
         <f t="shared" si="3"/>
         <v>1308</v>
@@ -5841,7 +5875,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:7">
       <c r="A140">
         <f t="shared" si="3"/>
         <v>1317</v>
@@ -5859,7 +5893,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:7">
       <c r="A141">
         <f t="shared" si="3"/>
         <v>1345</v>
@@ -5877,7 +5911,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:7">
       <c r="A142">
         <f t="shared" si="3"/>
         <v>1350</v>
@@ -5895,7 +5929,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:7">
       <c r="A143">
         <f t="shared" si="3"/>
         <v>1367</v>
@@ -5913,7 +5947,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:7">
       <c r="A144">
         <f t="shared" si="3"/>
         <v>1384</v>
@@ -6102,10 +6136,13 @@
         <v>350</v>
       </c>
       <c r="D155" t="s">
-        <v>719</v>
+        <v>641</v>
       </c>
       <c r="E155" t="s">
         <v>727</v>
+      </c>
+      <c r="G155" s="68" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -7013,7 +7050,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:7">
       <c r="A209">
         <f t="shared" si="5"/>
         <v>3708</v>
@@ -7031,7 +7068,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:7">
       <c r="A210">
         <f t="shared" si="5"/>
         <v>3718</v>
@@ -7046,7 +7083,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:7">
       <c r="A211">
         <f t="shared" si="5"/>
         <v>3746</v>
@@ -7061,7 +7098,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:7">
       <c r="A212">
         <f t="shared" si="5"/>
         <v>3756</v>
@@ -7079,7 +7116,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:7">
       <c r="A213">
         <f t="shared" si="5"/>
         <v>3766</v>
@@ -7094,7 +7131,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:7">
       <c r="A214">
         <v>3773</v>
       </c>
@@ -7108,7 +7145,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="215" spans="1:6">
+    <row r="215" spans="1:7">
       <c r="A215">
         <v>3823</v>
       </c>
@@ -7122,7 +7159,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="216" spans="1:6">
+    <row r="216" spans="1:7">
       <c r="A216">
         <v>3851</v>
       </c>
@@ -7136,7 +7173,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:7">
       <c r="A217">
         <v>3853</v>
       </c>
@@ -7146,11 +7183,11 @@
       <c r="C217" t="s">
         <v>500</v>
       </c>
-      <c r="D217" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6">
+      <c r="G217" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
       <c r="A218">
         <v>3881</v>
       </c>
@@ -7164,7 +7201,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="219" spans="1:6">
+    <row r="219" spans="1:7">
       <c r="A219">
         <v>3890</v>
       </c>
@@ -7181,7 +7218,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:7">
       <c r="A220">
         <v>3898</v>
       </c>
@@ -7198,7 +7235,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:7">
       <c r="A221">
         <v>3902</v>
       </c>
@@ -7212,7 +7249,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="222" spans="1:6">
+    <row r="222" spans="1:7">
       <c r="A222">
         <v>3952</v>
       </c>
@@ -7226,7 +7263,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="223" spans="1:6">
+    <row r="223" spans="1:7">
       <c r="A223">
         <v>4002</v>
       </c>
@@ -7240,7 +7277,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="224" spans="1:6">
+    <row r="224" spans="1:7">
       <c r="A224">
         <v>4052</v>
       </c>
@@ -7402,8 +7439,9 @@
       <c r="C234" t="s">
         <v>538</v>
       </c>
-      <c r="D234" t="s">
-        <v>717</v>
+      <c r="D234" s="68"/>
+      <c r="G234" s="68" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="235" spans="1:7">
@@ -7505,8 +7543,8 @@
       <c r="D240" t="s">
         <v>630</v>
       </c>
-      <c r="F240" t="s">
-        <v>706</v>
+      <c r="F240" s="68" t="s">
+        <v>702</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -7522,8 +7560,8 @@
       <c r="D241" s="68" t="s">
         <v>630</v>
       </c>
-      <c r="F241" t="s">
-        <v>706</v>
+      <c r="F241" s="68" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="242" spans="1:6">
@@ -7982,7 +8020,7 @@
       <c r="K3" s="13"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="42">
+    <row r="4" spans="1:12" ht="14">
       <c r="A4" s="5">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
@@ -8010,7 +8048,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="56">
+    <row r="5" spans="1:12" ht="28">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8041,7 +8079,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="56">
+    <row r="6" spans="1:12" ht="28">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8069,7 +8107,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="84">
+    <row r="7" spans="1:12" ht="42">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8150,7 +8188,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28">
+    <row r="10" spans="1:12" ht="14">
       <c r="A10" s="5">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8203,7 +8241,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="56">
+    <row r="12" spans="1:12" ht="28">
       <c r="A12" s="5">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -8287,7 +8325,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="70">
+    <row r="15" spans="1:12" ht="42">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8318,7 +8356,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="56">
+    <row r="16" spans="1:12" ht="28">
       <c r="A16" s="5">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8346,7 +8384,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="112">
+    <row r="17" spans="1:12" ht="84">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -8374,7 +8412,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="266">
+    <row r="18" spans="1:12" ht="168">
       <c r="A18" s="5">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -8402,7 +8440,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="70">
+    <row r="19" spans="1:12" ht="42">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -8433,7 +8471,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="42">
+    <row r="20" spans="1:12" ht="14">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -8489,7 +8527,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28">
+    <row r="22" spans="1:12" ht="14">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -8517,7 +8555,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="42">
+    <row r="23" spans="1:12" ht="14">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -8579,7 +8617,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="13"/>
     </row>
-    <row r="25" spans="1:12" ht="42">
+    <row r="25" spans="1:12" ht="14">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -8607,7 +8645,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="42">
+    <row r="26" spans="1:12" ht="14">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -8726,7 +8764,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="126">
+    <row r="30" spans="1:12" ht="84">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8754,7 +8792,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="140">
+    <row r="31" spans="1:12" ht="84">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8813,7 +8851,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="140">
+    <row r="33" spans="1:11" ht="56">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -8844,7 +8882,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="126">
+    <row r="34" spans="1:11" ht="98">
       <c r="A34" s="5">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -8900,7 +8938,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="28">
+    <row r="36" spans="1:11" ht="14">
       <c r="A36" s="5">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -8990,7 +9028,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="182">
+    <row r="39" spans="1:11" ht="98">
       <c r="A39" s="5">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -9021,7 +9059,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="70">
+    <row r="40" spans="1:11" ht="42">
       <c r="A40" s="5">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -9052,7 +9090,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="70">
+    <row r="41" spans="1:11" ht="42">
       <c r="A41" s="5">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -9083,7 +9121,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="70">
+    <row r="42" spans="1:11" ht="42">
       <c r="A42" s="5">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -9114,7 +9152,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="70">
+    <row r="43" spans="1:11" ht="42">
       <c r="A43" s="5">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9176,7 +9214,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="84">
+    <row r="45" spans="1:11" ht="28">
       <c r="A45" s="5">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9820,7 +9858,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="70">
+    <row r="68" spans="1:11" ht="42">
       <c r="A68" s="5">
         <f t="shared" ref="A68:A100" si="2">A67+1</f>
         <v>67</v>
@@ -9832,7 +9870,7 @@
       <c r="C68" s="6">
         <v>3</v>
       </c>
-      <c r="D68" s="69" t="s">
+      <c r="D68" s="70" t="s">
         <v>168</v>
       </c>
       <c r="E68" s="8" t="s">
@@ -9863,7 +9901,7 @@
       <c r="C69" s="6">
         <v>3</v>
       </c>
-      <c r="D69" s="69"/>
+      <c r="D69" s="70"/>
       <c r="E69" s="8" t="s">
         <v>171</v>
       </c>
@@ -9892,7 +9930,7 @@
       <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="D70" s="69"/>
+      <c r="D70" s="70"/>
       <c r="E70" s="8" t="s">
         <v>173</v>
       </c>
@@ -9921,7 +9959,7 @@
       <c r="C71" s="6">
         <v>3</v>
       </c>
-      <c r="D71" s="69"/>
+      <c r="D71" s="70"/>
       <c r="E71" s="8" t="s">
         <v>174</v>
       </c>
@@ -9950,7 +9988,7 @@
       <c r="C72" s="6">
         <v>3</v>
       </c>
-      <c r="D72" s="69"/>
+      <c r="D72" s="70"/>
       <c r="E72" s="8" t="s">
         <v>175</v>
       </c>
@@ -9979,7 +10017,7 @@
       <c r="C73" s="6">
         <v>3</v>
       </c>
-      <c r="D73" s="69"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="8" t="s">
         <v>176</v>
       </c>
@@ -10008,7 +10046,7 @@
       <c r="C74" s="6">
         <v>3</v>
       </c>
-      <c r="D74" s="69"/>
+      <c r="D74" s="70"/>
       <c r="E74" s="8" t="s">
         <v>177</v>
       </c>
@@ -10037,7 +10075,7 @@
       <c r="C75" s="6">
         <v>3</v>
       </c>
-      <c r="D75" s="69"/>
+      <c r="D75" s="70"/>
       <c r="E75" s="8" t="s">
         <v>178</v>
       </c>
@@ -10066,7 +10104,7 @@
       <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="D76" s="69"/>
+      <c r="D76" s="70"/>
       <c r="E76" s="8" t="s">
         <v>179</v>
       </c>
@@ -10095,7 +10133,7 @@
       <c r="C77" s="6">
         <v>3</v>
       </c>
-      <c r="D77" s="69"/>
+      <c r="D77" s="70"/>
       <c r="E77" s="8" t="s">
         <v>180</v>
       </c>
@@ -10124,7 +10162,7 @@
       <c r="C78" s="6">
         <v>3</v>
       </c>
-      <c r="D78" s="69"/>
+      <c r="D78" s="70"/>
       <c r="E78" s="8" t="s">
         <v>181</v>
       </c>
@@ -10153,7 +10191,7 @@
       <c r="C79" s="6">
         <v>3</v>
       </c>
-      <c r="D79" s="69"/>
+      <c r="D79" s="70"/>
       <c r="E79" s="8" t="s">
         <v>182</v>
       </c>
@@ -10182,7 +10220,7 @@
       <c r="C80" s="6">
         <v>3</v>
       </c>
-      <c r="D80" s="69"/>
+      <c r="D80" s="70"/>
       <c r="E80" s="8" t="s">
         <v>183</v>
       </c>
@@ -10211,7 +10249,7 @@
       <c r="C81" s="6">
         <v>3</v>
       </c>
-      <c r="D81" s="69"/>
+      <c r="D81" s="70"/>
       <c r="E81" s="8" t="s">
         <v>184</v>
       </c>
@@ -10240,7 +10278,7 @@
       <c r="C82" s="6">
         <v>3</v>
       </c>
-      <c r="D82" s="69"/>
+      <c r="D82" s="70"/>
       <c r="E82" s="8" t="s">
         <v>185</v>
       </c>
@@ -10269,7 +10307,7 @@
       <c r="C83" s="6">
         <v>3</v>
       </c>
-      <c r="D83" s="69"/>
+      <c r="D83" s="70"/>
       <c r="E83" s="8" t="s">
         <v>186</v>
       </c>
@@ -10286,7 +10324,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="70">
+    <row r="84" spans="1:11" ht="42">
       <c r="A84" s="5">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -10346,7 +10384,7 @@
       <c r="J85" s="20"/>
       <c r="K85" s="23"/>
     </row>
-    <row r="86" spans="1:11" ht="182">
+    <row r="86" spans="1:11" ht="70">
       <c r="A86" s="5">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -10406,7 +10444,7 @@
       <c r="J87" s="20"/>
       <c r="K87" s="23"/>
     </row>
-    <row r="88" spans="1:11" ht="182">
+    <row r="88" spans="1:11" ht="70">
       <c r="A88" s="5">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -10439,7 +10477,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="56">
+    <row r="89" spans="1:11" ht="28">
       <c r="A89" s="5">
         <f t="shared" si="2"/>
         <v>88</v>
@@ -10470,7 +10508,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="98">
+    <row r="90" spans="1:11" ht="56">
       <c r="A90" s="5">
         <f t="shared" si="2"/>
         <v>89</v>
@@ -10529,7 +10567,7 @@
       <c r="J91" s="12"/>
       <c r="K91" s="13"/>
     </row>
-    <row r="92" spans="1:11" ht="42">
+    <row r="92" spans="1:11" ht="14">
       <c r="A92" s="5">
         <f t="shared" si="2"/>
         <v>91</v>
@@ -10689,7 +10727,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="154">
+    <row r="97" spans="1:12" ht="56">
       <c r="A97" s="5">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -10748,7 +10786,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="42">
+    <row r="99" spans="1:12" ht="28">
       <c r="A99" s="5">
         <f t="shared" si="2"/>
         <v>98</v>
@@ -10830,7 +10868,7 @@
       <c r="F101" s="22" t="s">
         <v>685</v>
       </c>
-      <c r="G101" s="70" t="s">
+      <c r="G101" s="71" t="s">
         <v>227</v>
       </c>
       <c r="H101" s="20" t="s">
@@ -10861,7 +10899,7 @@
       <c r="F102" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G102" s="70"/>
+      <c r="G102" s="71"/>
       <c r="H102" s="33"/>
       <c r="I102" s="7" t="s">
         <v>706</v>
@@ -10893,7 +10931,7 @@
       <c r="F103" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G103" s="70"/>
+      <c r="G103" s="71"/>
       <c r="H103" s="33"/>
       <c r="I103" s="7" t="s">
         <v>706</v>
@@ -10924,7 +10962,7 @@
       <c r="F104" s="22" t="s">
         <v>686</v>
       </c>
-      <c r="G104" s="70"/>
+      <c r="G104" s="71"/>
       <c r="H104" s="20" t="s">
         <v>727</v>
       </c>
@@ -10955,7 +10993,7 @@
       <c r="F105" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="G105" s="70"/>
+      <c r="G105" s="71"/>
       <c r="H105" s="20" t="s">
         <v>727</v>
       </c>
@@ -10984,7 +11022,7 @@
       <c r="F106" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G106" s="70"/>
+      <c r="G106" s="71"/>
       <c r="H106" s="33"/>
       <c r="I106" s="33" t="s">
         <v>706</v>
@@ -11015,7 +11053,7 @@
       <c r="F107" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G107" s="70"/>
+      <c r="G107" s="71"/>
       <c r="H107" s="33"/>
       <c r="I107" s="33" t="s">
         <v>706</v>
@@ -11046,7 +11084,7 @@
       <c r="F108" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="G108" s="70"/>
+      <c r="G108" s="71"/>
       <c r="H108" s="33"/>
       <c r="I108" s="33" t="s">
         <v>706</v>
@@ -11077,7 +11115,7 @@
       <c r="F109" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="G109" s="70"/>
+      <c r="G109" s="71"/>
       <c r="H109" s="20" t="s">
         <v>727</v>
       </c>
@@ -11108,7 +11146,7 @@
       <c r="F110" s="22" t="s">
         <v>689</v>
       </c>
-      <c r="G110" s="70"/>
+      <c r="G110" s="71"/>
       <c r="H110" s="20" t="s">
         <v>727</v>
       </c>
@@ -11137,7 +11175,7 @@
       <c r="F111" s="22" t="s">
         <v>690</v>
       </c>
-      <c r="G111" s="70"/>
+      <c r="G111" s="71"/>
       <c r="H111" s="20" t="s">
         <v>727</v>
       </c>
@@ -11166,7 +11204,7 @@
       <c r="F112" s="22" t="s">
         <v>691</v>
       </c>
-      <c r="G112" s="70"/>
+      <c r="G112" s="71"/>
       <c r="H112" s="20" t="s">
         <v>727</v>
       </c>
@@ -11195,7 +11233,7 @@
       <c r="F113" s="22" t="s">
         <v>692</v>
       </c>
-      <c r="G113" s="70"/>
+      <c r="G113" s="71"/>
       <c r="H113" s="20" t="s">
         <v>727</v>
       </c>
@@ -11224,7 +11262,7 @@
       <c r="F114" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G114" s="70"/>
+      <c r="G114" s="71"/>
       <c r="H114" s="33"/>
       <c r="I114" s="33" t="s">
         <v>706</v>
@@ -11253,7 +11291,7 @@
       <c r="F115" s="22" t="s">
         <v>693</v>
       </c>
-      <c r="G115" s="70"/>
+      <c r="G115" s="71"/>
       <c r="H115" s="20" t="s">
         <v>727</v>
       </c>
@@ -11282,7 +11320,7 @@
       <c r="F116" s="22" t="s">
         <v>694</v>
       </c>
-      <c r="G116" s="70"/>
+      <c r="G116" s="71"/>
       <c r="H116" s="20" t="s">
         <v>727</v>
       </c>
@@ -11311,7 +11349,7 @@
       <c r="F117" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="G117" s="70"/>
+      <c r="G117" s="71"/>
       <c r="H117" s="20"/>
       <c r="I117" s="33">
         <v>2022</v>
@@ -11342,7 +11380,7 @@
       <c r="F118" s="22" t="s">
         <v>695</v>
       </c>
-      <c r="G118" s="70"/>
+      <c r="G118" s="71"/>
       <c r="H118" s="20" t="s">
         <v>727</v>
       </c>
@@ -11371,7 +11409,7 @@
       <c r="F119" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="G119" s="70"/>
+      <c r="G119" s="71"/>
       <c r="H119" s="20" t="s">
         <v>727</v>
       </c>
@@ -11400,7 +11438,7 @@
       <c r="F120" s="22" t="s">
         <v>696</v>
       </c>
-      <c r="G120" s="70"/>
+      <c r="G120" s="71"/>
       <c r="H120" s="20" t="s">
         <v>727</v>
       </c>
@@ -11429,7 +11467,7 @@
       <c r="F121" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G121" s="70"/>
+      <c r="G121" s="71"/>
       <c r="H121" s="33"/>
       <c r="I121" s="33" t="s">
         <v>706</v>
@@ -11459,7 +11497,7 @@
       <c r="F122" s="64" t="s">
         <v>630</v>
       </c>
-      <c r="G122" s="70"/>
+      <c r="G122" s="71"/>
       <c r="H122" s="33"/>
       <c r="I122" s="33" t="s">
         <v>706</v>
@@ -11467,7 +11505,7 @@
       <c r="J122" s="33"/>
       <c r="K122" s="34"/>
     </row>
-    <row r="123" spans="1:12" ht="182">
+    <row r="123" spans="1:12" ht="70">
       <c r="A123" s="5">
         <f t="shared" si="4"/>
         <v>122</v>
@@ -11499,7 +11537,7 @@
       <c r="K123" s="23"/>
       <c r="L123" s="7"/>
     </row>
-    <row r="124" spans="1:12" ht="28">
+    <row r="124" spans="1:12" ht="14">
       <c r="A124" s="5">
         <f t="shared" si="4"/>
         <v>123</v>
@@ -11531,7 +11569,7 @@
       <c r="K124" s="23"/>
       <c r="L124" s="7"/>
     </row>
-    <row r="125" spans="1:12" ht="42">
+    <row r="125" spans="1:12" ht="14">
       <c r="A125" s="5">
         <f t="shared" si="4"/>
         <v>124</v>
@@ -11563,7 +11601,7 @@
       <c r="K125" s="23"/>
       <c r="L125" s="7"/>
     </row>
-    <row r="126" spans="1:12" ht="56">
+    <row r="126" spans="1:12" ht="28">
       <c r="A126" s="5">
         <f t="shared" si="4"/>
         <v>125</v>
@@ -11595,7 +11633,7 @@
       <c r="K126" s="23"/>
       <c r="L126" s="7"/>
     </row>
-    <row r="127" spans="1:12" ht="42">
+    <row r="127" spans="1:12" ht="14">
       <c r="A127" s="5">
         <f t="shared" si="4"/>
         <v>126</v>
@@ -11653,7 +11691,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="28">
+    <row r="129" spans="1:11" ht="14">
       <c r="A129" s="5">
         <f>A128+1</f>
         <v>128</v>
@@ -11681,7 +11719,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="98">
+    <row r="130" spans="1:11" ht="42">
       <c r="A130" s="5">
         <f>A129+1</f>
         <v>129</v>
@@ -11865,7 +11903,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="42">
+    <row r="137" spans="1:11" ht="14">
       <c r="A137" s="5">
         <f t="shared" si="7"/>
         <v>136</v>
@@ -11893,7 +11931,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="70">
+    <row r="138" spans="1:11" ht="28">
       <c r="A138" s="5">
         <f t="shared" si="7"/>
         <v>137</v>
@@ -11921,7 +11959,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="112">
+    <row r="139" spans="1:11" ht="42">
       <c r="A139" s="5">
         <f t="shared" si="7"/>
         <v>138</v>
@@ -11949,7 +11987,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="28">
+    <row r="140" spans="1:11" ht="14">
       <c r="A140" s="5">
         <f t="shared" si="7"/>
         <v>139</v>
@@ -12061,7 +12099,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="70">
+    <row r="144" spans="1:11" ht="42">
       <c r="A144" s="5">
         <f t="shared" si="7"/>
         <v>143</v>
@@ -12089,7 +12127,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="56">
+    <row r="145" spans="1:11" ht="28">
       <c r="A145" s="5">
         <f t="shared" si="7"/>
         <v>144</v>
@@ -12117,7 +12155,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="56">
+    <row r="146" spans="1:11" ht="28">
       <c r="A146" s="5">
         <f t="shared" si="7"/>
         <v>145</v>
@@ -12319,7 +12357,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="42">
+    <row r="153" spans="1:11" ht="28">
       <c r="A153" s="5">
         <f t="shared" si="7"/>
         <v>152</v>
@@ -12414,7 +12452,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="70">
+    <row r="156" spans="1:11" ht="28">
       <c r="A156" s="5">
         <f t="shared" si="7"/>
         <v>155</v>
@@ -12443,7 +12481,7 @@
       <c r="J156" s="20"/>
       <c r="K156" s="23"/>
     </row>
-    <row r="157" spans="1:11" ht="42">
+    <row r="157" spans="1:11" ht="28">
       <c r="A157" s="5">
         <f t="shared" si="7"/>
         <v>156</v>
@@ -12701,7 +12739,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="70">
+    <row r="166" spans="1:11" ht="28">
       <c r="A166" s="5">
         <f t="shared" si="7"/>
         <v>165</v>
@@ -12938,7 +12976,7 @@
       <c r="J174" s="20"/>
       <c r="K174" s="23"/>
     </row>
-    <row r="175" spans="1:11" ht="56">
+    <row r="175" spans="1:11" ht="28">
       <c r="A175" s="5">
         <f t="shared" si="7"/>
         <v>174</v>
@@ -13000,7 +13038,7 @@
       <c r="J176" s="20"/>
       <c r="K176" s="23"/>
     </row>
-    <row r="177" spans="1:12" ht="42">
+    <row r="177" spans="1:12" ht="28">
       <c r="A177" s="5">
         <f t="shared" si="7"/>
         <v>176</v>
@@ -13028,7 +13066,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="84">
+    <row r="178" spans="1:12" ht="42">
       <c r="A178" s="5">
         <f t="shared" si="7"/>
         <v>177</v>
@@ -13056,7 +13094,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="42">
+    <row r="179" spans="1:12" ht="28">
       <c r="A179" s="5">
         <f t="shared" si="7"/>
         <v>178</v>
@@ -13084,7 +13122,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="70">
+    <row r="180" spans="1:12" ht="28">
       <c r="A180" s="5">
         <f t="shared" si="7"/>
         <v>179</v>
@@ -13199,7 +13237,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="224">
+    <row r="184" spans="1:12" ht="112">
       <c r="A184" s="5">
         <f t="shared" si="7"/>
         <v>183</v>
@@ -13231,7 +13269,7 @@
       <c r="K184" s="49"/>
       <c r="L184" s="7"/>
     </row>
-    <row r="185" spans="1:12" ht="98">
+    <row r="185" spans="1:12" ht="28">
       <c r="A185" s="5">
         <f t="shared" si="7"/>
         <v>184</v>
@@ -13571,7 +13609,7 @@
       <c r="J195" s="9"/>
       <c r="K195" s="54"/>
     </row>
-    <row r="196" spans="1:11" ht="42">
+    <row r="196" spans="1:11" ht="14">
       <c r="A196" s="5">
         <f t="shared" si="10"/>
         <v>195</v>
@@ -13786,7 +13824,7 @@
       <c r="J203" s="12"/>
       <c r="K203" s="13"/>
     </row>
-    <row r="204" spans="1:11" ht="84">
+    <row r="204" spans="1:11" ht="28">
       <c r="A204" s="5">
         <f t="shared" si="10"/>
         <v>203</v>
@@ -13816,7 +13854,7 @@
       <c r="J204" s="24"/>
       <c r="K204" s="25"/>
     </row>
-    <row r="205" spans="1:11" ht="42">
+    <row r="205" spans="1:11" ht="14">
       <c r="A205" s="5">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -13871,7 +13909,7 @@
       <c r="J206" s="9"/>
       <c r="K206" s="54"/>
     </row>
-    <row r="207" spans="1:11" ht="42">
+    <row r="207" spans="1:11" ht="28">
       <c r="A207" s="5">
         <f t="shared" si="10"/>
         <v>206</v>
@@ -14036,7 +14074,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="319">
+    <row r="214" spans="1:11" ht="112">
       <c r="A214" s="5">
         <f t="shared" si="10"/>
         <v>213</v>
@@ -14116,7 +14154,7 @@
       <c r="J216" s="12"/>
       <c r="K216" s="13"/>
     </row>
-    <row r="217" spans="1:11" ht="84">
+    <row r="217" spans="1:11" ht="28">
       <c r="A217" s="5">
         <f t="shared" si="10"/>
         <v>216</v>
@@ -14144,7 +14182,7 @@
       <c r="J217" s="24"/>
       <c r="K217" s="25"/>
     </row>
-    <row r="218" spans="1:11" ht="112">
+    <row r="218" spans="1:11" ht="42">
       <c r="A218" s="5">
         <f t="shared" si="10"/>
         <v>217</v>
@@ -14168,7 +14206,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="28">
+    <row r="219" spans="1:11" ht="14">
       <c r="A219" s="5">
         <f t="shared" si="10"/>
         <v>218</v>
@@ -14495,7 +14533,7 @@
       <c r="J231" s="37"/>
       <c r="K231" s="38"/>
     </row>
-    <row r="232" spans="1:11" ht="42">
+    <row r="232" spans="1:11" ht="14">
       <c r="A232" s="5">
         <f t="shared" si="10"/>
         <v>231</v>
@@ -14547,7 +14585,7 @@
       <c r="J233" s="12"/>
       <c r="K233" s="13"/>
     </row>
-    <row r="234" spans="1:11" ht="70">
+    <row r="234" spans="1:11" ht="28">
       <c r="A234" s="5">
         <f t="shared" si="10"/>
         <v>233</v>
@@ -14575,7 +14613,7 @@
       <c r="J234" s="12"/>
       <c r="K234" s="13"/>
     </row>
-    <row r="235" spans="1:11" ht="112">
+    <row r="235" spans="1:11" ht="42">
       <c r="A235" s="5">
         <f t="shared" si="10"/>
         <v>234</v>
@@ -14629,7 +14667,7 @@
       <c r="J236" s="9"/>
       <c r="K236" s="54"/>
     </row>
-    <row r="237" spans="1:11" ht="56">
+    <row r="237" spans="1:11" ht="28">
       <c r="A237" s="5">
         <f t="shared" si="10"/>
         <v>236</v>
@@ -14656,7 +14694,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="98">
+    <row r="238" spans="1:11" ht="42">
       <c r="A238" s="5">
         <f t="shared" si="10"/>
         <v>237</v>
@@ -14686,7 +14724,7 @@
       <c r="J238" s="24"/>
       <c r="K238" s="25"/>
     </row>
-    <row r="239" spans="1:11" ht="84">
+    <row r="239" spans="1:11" ht="28">
       <c r="A239" s="5">
         <f t="shared" si="10"/>
         <v>238</v>
@@ -14716,7 +14754,7 @@
       <c r="J239" s="24"/>
       <c r="K239" s="25"/>
     </row>
-    <row r="240" spans="1:11" ht="42">
+    <row r="240" spans="1:11" ht="14">
       <c r="A240" s="5">
         <f t="shared" si="10"/>
         <v>239</v>
@@ -14744,7 +14782,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="42">
+    <row r="241" spans="1:11" ht="14">
       <c r="A241" s="5">
         <f t="shared" si="10"/>
         <v>240</v>
@@ -14771,7 +14809,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="56">
+    <row r="242" spans="1:11" ht="28">
       <c r="A242" s="5">
         <f t="shared" si="10"/>
         <v>241</v>
@@ -14798,7 +14836,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="28">
+    <row r="243" spans="1:11" ht="14">
       <c r="A243" s="5">
         <f t="shared" si="10"/>
         <v>242</v>
@@ -14852,7 +14890,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="28">
+    <row r="245" spans="1:11" ht="14">
       <c r="A245" s="5">
         <f t="shared" si="10"/>
         <v>244</v>
@@ -14879,7 +14917,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="246" spans="1:11" ht="42">
+    <row r="246" spans="1:11" ht="14">
       <c r="A246" s="5">
         <f t="shared" si="10"/>
         <v>245</v>
@@ -15257,7 +15295,7 @@
       <c r="J258" s="62"/>
       <c r="K258" s="63"/>
     </row>
-    <row r="259" spans="1:11" ht="70">
+    <row r="259" spans="1:11" ht="28">
       <c r="A259" s="5">
         <f t="shared" ref="A259:A260" si="13">A258+1</f>
         <v>258</v>
@@ -15284,7 +15322,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="98">
+    <row r="260" spans="1:11" ht="28">
       <c r="A260" s="5">
         <f t="shared" si="13"/>
         <v>259</v>

</xml_diff>

<commit_message>
Correct mapping for year of injury
</commit_message>
<xml_diff>
--- a/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
+++ b/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rscalfani/Documents/code/NVSS/vrdr-dotnet/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krautscheid/git/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DF61D8-C191-B242-8B05-63C2DCE89612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D5611D-4C67-4A4E-A2C6-8BC5C21053EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="764">
   <si>
     <t>Field #</t>
   </si>
@@ -2670,6 +2670,9 @@
   </si>
   <si>
     <t>use_2022_if_no_injury</t>
+  </si>
+  <si>
+    <t>Injury Date year</t>
   </si>
 </sst>
 </file>
@@ -3032,7 +3035,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3354,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD74E696-0F05-DF43-9EB9-28DAB6A6F493}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G117" sqref="G117"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5473,6 +5476,12 @@
       </c>
       <c r="C117" t="s">
         <v>259</v>
+      </c>
+      <c r="D117" s="68" t="s">
+        <v>763</v>
+      </c>
+      <c r="E117" s="68" t="s">
+        <v>727</v>
       </c>
       <c r="G117" s="68" t="s">
         <v>762</v>
@@ -15386,10 +15395,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d8a0f530da2fdbe2e55626e9ad23fb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d278552e3c3a0a08e9db34919b560943" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -15611,35 +15636,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0A455F-891F-4D48-ABA8-1B564ACEA7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15659,21 +15679,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More improvements to tabular data importer
</commit_message>
<xml_diff>
--- a/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
+++ b/tools/IJE_File_Layouts_Tabular_Input_Mapping_Version_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krautscheid/git/vrdr-dotnet/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D5611D-4C67-4A4E-A2C6-8BC5C21053EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1076B6-4331-6C47-B355-9D5F56E19D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="28300" tabRatio="779" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="764">
   <si>
     <t>Field #</t>
   </si>
@@ -3357,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD74E696-0F05-DF43-9EB9-28DAB6A6F493}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3627,8 +3627,8 @@
       <c r="D15" t="s">
         <v>630</v>
       </c>
-      <c r="F15" t="s">
-        <v>706</v>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -3696,8 +3696,8 @@
       <c r="D19" t="s">
         <v>630</v>
       </c>
-      <c r="F19" t="s">
-        <v>706</v>
+      <c r="F19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3915,8 +3915,8 @@
       <c r="D31" t="s">
         <v>630</v>
       </c>
-      <c r="F31" t="s">
-        <v>706</v>
+      <c r="F31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -4059,8 +4059,8 @@
       <c r="D39" t="s">
         <v>630</v>
       </c>
-      <c r="F39" t="s">
-        <v>706</v>
+      <c r="F39">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5426,8 +5426,8 @@
       <c r="D114" t="s">
         <v>630</v>
       </c>
-      <c r="F114" t="s">
-        <v>706</v>
+      <c r="F114">
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -7915,7 +7915,7 @@
   <dimension ref="A1:L1048511"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="95" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -15395,26 +15395,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002752A2C1F044FE469AAF2142AB326B8C" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d8a0f530da2fdbe2e55626e9ad23fb0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1a58edb-1ba6-4800-9942-1e1defaa36d6" xmlns:ns3="4b113022-9134-4b2e-abe8-26e86c9e296e" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d278552e3c3a0a08e9db34919b560943" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
@@ -15636,30 +15620,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c1a58edb-1ba6-4800-9942-1e1defaa36d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C0A455F-891F-4D48-ABA8-1B564ACEA7DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15679,10 +15668,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D8D0BD-9993-4EC8-86D1-0A7C5F6E1934}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6E1C13E-614F-4B48-A9FE-F6158F0F568F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{370C49E3-78D0-405B-AC39-DEC8FE68C756}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="c1a58edb-1ba6-4800-9942-1e1defaa36d6"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>